<commit_message>
Multi Layer NN implemented
</commit_message>
<xml_diff>
--- a/Datasheets.xlsx
+++ b/Datasheets.xlsx
@@ -141,6 +141,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -856,6 +857,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -946,11 +948,12 @@
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Percent Change</a:t>
+                  <a:t>Percent Noise</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5987,7 +5990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -6812,7 +6817,7 @@
   <dimension ref="A1:C303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>